<commit_message>
Change date in rebate2 file
</commit_message>
<xml_diff>
--- a/ge-empower-autotests/src/test/resources/testdata/rebate2.xlsx
+++ b/ge-empower-autotests/src/test/resources/testdata/rebate2.xlsx
@@ -67,7 +67,7 @@
     <t xml:space="preserve">TEST</t>
   </si>
   <si>
-    <t xml:space="preserve">08/27/2018</t>
+    <t xml:space="preserve">11/25/2018</t>
   </si>
 </sst>
 </file>
@@ -274,9 +274,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1189080</xdr:colOff>
+      <xdr:colOff>1188720</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>160560</xdr:rowOff>
+      <xdr:rowOff>160200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -290,7 +290,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="1189080" cy="922320"/>
+          <a:ext cx="1188720" cy="921960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -312,7 +312,7 @@
   </sheetPr>
   <dimension ref="A1:L7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G7" activeCellId="0" sqref="G7"/>
     </sheetView>
   </sheetViews>

</xml_diff>